<commit_message>
ADCC Template V2: Added transaction template tags and split into multiple tables based on victim account number sequence (not need to split for suspects because each ADCC is only for one suspect). Added Suspect Number for beneficiary details and {Fraud Payment, Located, Suspect Number, Victim Number, Victim Account Number Sequence} for txn details
</commit_message>
<xml_diff>
--- a/Raw Input Data/Template V2/ADCC V2.xlsx
+++ b/Raw Input Data/Template V2/ADCC V2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Documents\hase-scripts\Raw Input Data\Template V2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{220F828E-FF4D-4162-B01C-493BB4F19B15}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C7CB24E-841F-4130-968A-322459EB262A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="6690" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{D98D0E3F-6E76-754A-9BB6-79DE637B44FD}"/>
+    <workbookView xWindow="-28920" yWindow="6690" windowWidth="29040" windowHeight="15720" firstSheet="1" activeTab="2" xr2:uid="{D98D0E3F-6E76-754A-9BB6-79DE637B44FD}"/>
   </bookViews>
   <sheets>
     <sheet name="ADCC-Params" sheetId="1" r:id="rId1"/>
@@ -64,7 +64,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="111">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="175" uniqueCount="116">
   <si>
     <t>Value</t>
   </si>
@@ -409,6 +409,21 @@
   </si>
   <si>
     <t>Victim Account Number Sequence</t>
+  </si>
+  <si>
+    <t>Sections_of_table_of_beneficiary_details_with_tables_of_transaction_details</t>
+  </si>
+  <si>
+    <t>AC2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">111-111111-102 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">CHUNG SIU </t>
+  </si>
+  <si>
+    <t>Victim Number</t>
   </si>
 </sst>
 </file>
@@ -486,7 +501,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -499,14 +514,10 @@
     </xf>
     <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="4" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="4" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
@@ -847,7 +858,7 @@
   <dimension ref="A1:O13"/>
   <sheetViews>
     <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -868,27 +879,24 @@
       <c r="A2" t="s">
         <v>11</v>
       </c>
-      <c r="B2" s="9" t="s">
+      <c r="B2" s="2" t="s">
         <v>96</v>
       </c>
-      <c r="D2" s="9"/>
-      <c r="E2" s="9"/>
-      <c r="F2" s="9"/>
-      <c r="G2" s="8"/>
-      <c r="H2" s="8"/>
-      <c r="I2" s="10"/>
-      <c r="J2" s="10"/>
-      <c r="K2" s="9"/>
-      <c r="L2" s="8"/>
-      <c r="M2" s="9"/>
-      <c r="N2" s="11"/>
-      <c r="O2" s="9"/>
+      <c r="D2" s="2"/>
+      <c r="E2" s="2"/>
+      <c r="F2" s="2"/>
+      <c r="I2" s="8"/>
+      <c r="J2" s="8"/>
+      <c r="K2" s="2"/>
+      <c r="M2" s="2"/>
+      <c r="N2" s="9"/>
+      <c r="O2" s="2"/>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>12</v>
       </c>
-      <c r="B3" s="9" t="s">
+      <c r="B3" s="2" t="s">
         <v>97</v>
       </c>
     </row>
@@ -896,7 +904,7 @@
       <c r="A4" t="s">
         <v>13</v>
       </c>
-      <c r="B4" s="9" t="s">
+      <c r="B4" s="2" t="s">
         <v>98</v>
       </c>
     </row>
@@ -904,13 +912,13 @@
       <c r="A5" t="s">
         <v>14</v>
       </c>
-      <c r="B5" s="8"/>
+      <c r="B5"/>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>53</v>
       </c>
-      <c r="B6" s="8" t="s">
+      <c r="B6" t="s">
         <v>90</v>
       </c>
       <c r="D6" s="3"/>
@@ -919,7 +927,7 @@
       <c r="A7" t="s">
         <v>58</v>
       </c>
-      <c r="B7" s="10" t="s">
+      <c r="B7" s="8" t="s">
         <v>93</v>
       </c>
     </row>
@@ -927,7 +935,7 @@
       <c r="A8" t="s">
         <v>59</v>
       </c>
-      <c r="B8" s="10" t="s">
+      <c r="B8" s="8" t="s">
         <v>60</v>
       </c>
     </row>
@@ -935,7 +943,7 @@
       <c r="A9" t="s">
         <v>62</v>
       </c>
-      <c r="B9" s="9" t="s">
+      <c r="B9" s="2" t="s">
         <v>63</v>
       </c>
     </row>
@@ -943,7 +951,7 @@
       <c r="A10" t="s">
         <v>68</v>
       </c>
-      <c r="B10" s="8" t="s">
+      <c r="B10" t="s">
         <v>99</v>
       </c>
     </row>
@@ -951,7 +959,7 @@
       <c r="A11" t="s">
         <v>83</v>
       </c>
-      <c r="B11" s="9" t="s">
+      <c r="B11" s="2" t="s">
         <v>77</v>
       </c>
     </row>
@@ -959,7 +967,7 @@
       <c r="A12" t="s">
         <v>82</v>
       </c>
-      <c r="B12" s="11" t="s">
+      <c r="B12" s="9" t="s">
         <v>95</v>
       </c>
     </row>
@@ -967,7 +975,7 @@
       <c r="A13" t="s">
         <v>84</v>
       </c>
-      <c r="B13" s="9" t="s">
+      <c r="B13" s="2" t="s">
         <v>85</v>
       </c>
     </row>
@@ -978,10 +986,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FFDFC332-B76A-F243-9758-115119AF4083}">
-  <dimension ref="A1:G5"/>
+  <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -991,7 +999,7 @@
     <col min="5" max="5" width="33.625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>29</v>
       </c>
@@ -1007,12 +1015,11 @@
       <c r="E1" t="s">
         <v>33</v>
       </c>
-      <c r="F1" s="12" t="s">
+      <c r="F1" t="s">
         <v>109</v>
       </c>
-      <c r="G1" s="12"/>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
         <v>100</v>
       </c>
@@ -1032,17 +1039,34 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="D3"/>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>112</v>
+      </c>
+      <c r="B3" t="s">
+        <v>34</v>
+      </c>
+      <c r="C3" t="s">
+        <v>101</v>
+      </c>
+      <c r="D3" t="s">
+        <v>113</v>
+      </c>
+      <c r="E3" t="s">
+        <v>114</v>
+      </c>
+      <c r="F3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="5"/>
       <c r="B4" s="5"/>
       <c r="C4" s="5"/>
       <c r="D4" s="5"/>
       <c r="E4" s="5"/>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="5"/>
       <c r="B5" s="5"/>
       <c r="C5" s="5"/>
@@ -1056,10 +1080,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1160796E-BF6B-334E-B5BD-991CA2BB931A}">
-  <dimension ref="A1:L30"/>
+  <dimension ref="A1:N30"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="H11" sqref="H11"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="J6" sqref="J6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1074,7 +1098,7 @@
     <col min="9" max="9" width="17.125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>41</v>
       </c>
@@ -1102,42 +1126,48 @@
       <c r="I1" t="s">
         <v>49</v>
       </c>
-      <c r="J1" s="12" t="s">
+      <c r="J1" t="s">
         <v>107</v>
       </c>
       <c r="K1" t="s">
         <v>108</v>
       </c>
       <c r="L1" t="s">
+        <v>109</v>
+      </c>
+      <c r="M1" t="s">
+        <v>115</v>
+      </c>
+      <c r="N1" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A2" s="12">
-        <v>1</v>
-      </c>
-      <c r="B2" s="13" t="s">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" s="2" t="s">
         <v>102</v>
       </c>
-      <c r="C2" s="12" t="s">
+      <c r="C2" t="s">
         <v>51</v>
       </c>
-      <c r="D2" s="14">
+      <c r="D2" s="10">
         <v>50000</v>
       </c>
-      <c r="E2" s="14">
+      <c r="E2" s="10">
         <v>50000</v>
       </c>
-      <c r="F2" s="12" t="s">
+      <c r="F2" t="s">
         <v>92</v>
       </c>
-      <c r="G2" s="12" t="s">
+      <c r="G2" t="s">
         <v>50</v>
       </c>
-      <c r="H2" s="12" t="s">
+      <c r="H2" t="s">
         <v>103</v>
       </c>
-      <c r="I2" s="12" t="s">
+      <c r="I2" t="s">
         <v>104</v>
       </c>
       <c r="J2">
@@ -1149,33 +1179,39 @@
       <c r="L2">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A3" s="12">
+      <c r="M2">
+        <v>1</v>
+      </c>
+      <c r="N2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A3">
         <v>2</v>
       </c>
-      <c r="B3" s="13" t="s">
+      <c r="B3" s="2" t="s">
         <v>105</v>
       </c>
-      <c r="C3" s="12" t="s">
+      <c r="C3" t="s">
         <v>51</v>
       </c>
-      <c r="D3" s="14">
+      <c r="D3" s="10">
         <v>10000</v>
       </c>
-      <c r="E3" s="14">
+      <c r="E3" s="10">
         <v>10000</v>
       </c>
-      <c r="F3" s="12" t="s">
+      <c r="F3" t="s">
         <v>92</v>
       </c>
-      <c r="G3" s="12" t="s">
+      <c r="G3" t="s">
         <v>50</v>
       </c>
-      <c r="H3" s="12" t="s">
+      <c r="H3" t="s">
         <v>103</v>
       </c>
-      <c r="I3" s="12" t="s">
+      <c r="I3" t="s">
         <v>104</v>
       </c>
       <c r="J3">
@@ -1187,33 +1223,39 @@
       <c r="L3">
         <v>1</v>
       </c>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A4" s="12">
-        <v>1</v>
-      </c>
-      <c r="B4" s="13" t="s">
+      <c r="M3">
+        <v>1</v>
+      </c>
+      <c r="N3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>1</v>
+      </c>
+      <c r="B4" s="2" t="s">
         <v>102</v>
       </c>
-      <c r="C4" s="12" t="s">
+      <c r="C4" t="s">
         <v>51</v>
       </c>
-      <c r="D4" s="15">
+      <c r="D4" s="11">
         <v>31000</v>
       </c>
-      <c r="E4" s="15">
+      <c r="E4" s="11">
         <v>31000</v>
       </c>
-      <c r="F4" s="13" t="s">
+      <c r="F4" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="G4" s="12" t="s">
+      <c r="G4" t="s">
         <v>50</v>
       </c>
-      <c r="H4" s="12" t="s">
+      <c r="H4" t="s">
         <v>106</v>
       </c>
-      <c r="I4" s="12" t="s">
+      <c r="I4" t="s">
         <v>104</v>
       </c>
       <c r="J4">
@@ -1223,35 +1265,41 @@
         <v>23</v>
       </c>
       <c r="L4">
+        <v>1</v>
+      </c>
+      <c r="M4">
+        <v>1</v>
+      </c>
+      <c r="N4">
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A5" s="12">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A5">
         <v>2</v>
       </c>
-      <c r="B5" s="13" t="s">
+      <c r="B5" s="2" t="s">
         <v>105</v>
       </c>
-      <c r="C5" s="12" t="s">
+      <c r="C5" t="s">
         <v>51</v>
       </c>
-      <c r="D5" s="15">
+      <c r="D5" s="11">
         <v>50000</v>
       </c>
-      <c r="E5" s="15">
+      <c r="E5" s="11">
         <v>50000</v>
       </c>
-      <c r="F5" s="13" t="s">
+      <c r="F5" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="G5" s="12" t="s">
+      <c r="G5" t="s">
         <v>50</v>
       </c>
-      <c r="H5" s="12" t="s">
+      <c r="H5" t="s">
         <v>106</v>
       </c>
-      <c r="I5" s="12" t="s">
+      <c r="I5" t="s">
         <v>104</v>
       </c>
       <c r="J5">
@@ -1261,73 +1309,85 @@
         <v>23</v>
       </c>
       <c r="L5">
+        <v>1</v>
+      </c>
+      <c r="M5">
+        <v>1</v>
+      </c>
+      <c r="N5">
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A6" s="12">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A6">
         <v>3</v>
       </c>
-      <c r="B6" s="13" t="s">
+      <c r="B6" s="2" t="s">
         <v>105</v>
       </c>
-      <c r="C6" s="12" t="s">
+      <c r="C6" t="s">
         <v>51</v>
       </c>
-      <c r="D6" s="15">
+      <c r="D6" s="11">
         <v>60000</v>
       </c>
-      <c r="E6" s="15">
+      <c r="E6" s="11">
         <v>60000</v>
       </c>
-      <c r="F6" s="13" t="s">
+      <c r="F6" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="G6" s="12" t="s">
+      <c r="G6" t="s">
         <v>50</v>
       </c>
-      <c r="H6" s="12" t="s">
+      <c r="H6" t="s">
         <v>106</v>
       </c>
-      <c r="I6" s="12" t="s">
+      <c r="I6" t="s">
         <v>104</v>
       </c>
       <c r="J6">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="K6" t="s">
         <v>23</v>
       </c>
       <c r="L6">
+        <v>1</v>
+      </c>
+      <c r="M6">
+        <v>1</v>
+      </c>
+      <c r="N6">
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A7" s="12">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A7">
         <v>4</v>
       </c>
-      <c r="B7" s="13" t="s">
+      <c r="B7" s="2" t="s">
         <v>105</v>
       </c>
-      <c r="C7" s="12" t="s">
+      <c r="C7" t="s">
         <v>51</v>
       </c>
-      <c r="D7" s="15">
+      <c r="D7" s="11">
         <v>30000</v>
       </c>
-      <c r="E7" s="15">
+      <c r="E7" s="11">
         <v>30000</v>
       </c>
-      <c r="F7" s="13" t="s">
+      <c r="F7" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="G7" s="12" t="s">
+      <c r="G7" t="s">
         <v>50</v>
       </c>
-      <c r="H7" s="12" t="s">
+      <c r="H7" t="s">
         <v>106</v>
       </c>
-      <c r="I7" s="12" t="s">
+      <c r="I7" t="s">
         <v>104</v>
       </c>
       <c r="J7">
@@ -1337,31 +1397,36 @@
         <v>23</v>
       </c>
       <c r="L7">
+        <v>1</v>
+      </c>
+      <c r="M7">
+        <v>1</v>
+      </c>
+      <c r="N7">
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A8" s="12">
-        <v>1</v>
-      </c>
-      <c r="B8" s="13" t="s">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>1</v>
+      </c>
+      <c r="B8" s="2" t="s">
         <v>105</v>
       </c>
-      <c r="C8" s="12" t="s">
+      <c r="C8" t="s">
         <v>51</v>
       </c>
-      <c r="D8" s="15">
+      <c r="D8" s="11">
         <v>39000</v>
       </c>
-      <c r="E8" s="15">
+      <c r="E8" s="11">
         <v>39000</v>
       </c>
-      <c r="F8" s="13"/>
-      <c r="G8" s="12" t="s">
+      <c r="F8" s="2"/>
+      <c r="G8" t="s">
         <v>50</v>
       </c>
-      <c r="H8" s="12"/>
-      <c r="I8" s="12" t="s">
+      <c r="I8" t="s">
         <v>104</v>
       </c>
       <c r="J8">
@@ -1371,59 +1436,139 @@
         <v>23</v>
       </c>
       <c r="L8">
+        <v>1</v>
+      </c>
+      <c r="M8">
+        <v>1</v>
+      </c>
+      <c r="N8">
         <v>3</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="B9" s="2"/>
-      <c r="D9" s="6"/>
-      <c r="E9" s="6"/>
-      <c r="G9" s="2"/>
-      <c r="H9" s="2"/>
-    </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="B10" s="2"/>
-      <c r="D10" s="6"/>
-      <c r="E10" s="6"/>
-      <c r="G10" s="2"/>
-      <c r="H10" s="2"/>
-    </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>1</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="C9" t="s">
+        <v>51</v>
+      </c>
+      <c r="D9" s="11">
+        <v>50000</v>
+      </c>
+      <c r="E9" s="11">
+        <v>50000</v>
+      </c>
+      <c r="F9" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="G9" t="s">
+        <v>50</v>
+      </c>
+      <c r="H9" t="s">
+        <v>103</v>
+      </c>
+      <c r="I9" t="s">
+        <v>104</v>
+      </c>
+      <c r="J9">
+        <v>9</v>
+      </c>
+      <c r="K9" t="s">
+        <v>23</v>
+      </c>
+      <c r="L9">
+        <v>2</v>
+      </c>
+      <c r="M9">
+        <v>1</v>
+      </c>
+      <c r="N9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>1</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="C10" t="s">
+        <v>51</v>
+      </c>
+      <c r="D10" s="6">
+        <v>50000</v>
+      </c>
+      <c r="E10" s="6">
+        <v>50000</v>
+      </c>
+      <c r="F10" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="G10" t="s">
+        <v>50</v>
+      </c>
+      <c r="H10" t="s">
+        <v>106</v>
+      </c>
+      <c r="I10" t="s">
+        <v>104</v>
+      </c>
+      <c r="J10">
+        <v>10</v>
+      </c>
+      <c r="K10" t="s">
+        <v>23</v>
+      </c>
+      <c r="L10">
+        <v>2</v>
+      </c>
+      <c r="M10">
+        <v>1</v>
+      </c>
+      <c r="N10">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B11" s="2"/>
       <c r="D11" s="6"/>
       <c r="E11" s="6"/>
       <c r="G11" s="2"/>
       <c r="H11" s="2"/>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B12" s="2"/>
       <c r="D12" s="6"/>
       <c r="E12" s="6"/>
       <c r="G12" s="2"/>
       <c r="H12" s="2"/>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B13" s="2"/>
       <c r="D13" s="6"/>
       <c r="E13" s="6"/>
       <c r="G13" s="2"/>
       <c r="H13" s="2"/>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B14" s="2"/>
       <c r="D14" s="6"/>
       <c r="E14" s="6"/>
       <c r="G14" s="2"/>
       <c r="H14" s="2"/>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B15" s="2"/>
       <c r="D15" s="6"/>
       <c r="E15" s="6"/>
       <c r="G15" s="2"/>
       <c r="H15" s="2"/>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B16" s="2"/>
       <c r="D16" s="6"/>
       <c r="E16" s="7"/>
@@ -1628,7 +1773,7 @@
     <row r="4" spans="1:3" ht="63" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="str" cm="1">
         <f t="array" ref="A4">"The details of next layer beneficiary account(s) relating to the below transaction of " &amp; "[" &amp; _xlfn.TEXTJOIN(", ", TRUE, IF('ADCC-Beneficiary-Details'!A2:'ADCC-Beneficiary-Details'!A10&lt;&gt;"", 'ADCC-Beneficiary-Details'!A2:'ADCC-Beneficiary-Details'!A10, "")) &amp; "]" &amp; " (including details of transaction, bank, account number and beneficiary name)."</f>
-        <v>The details of next layer beneficiary account(s) relating to the below transaction of [AC1] (including details of transaction, bank, account number and beneficiary name).</v>
+        <v>The details of next layer beneficiary account(s) relating to the below transaction of [AC1, AC2] (including details of transaction, bank, account number and beneficiary name).</v>
       </c>
       <c r="B4" t="s">
         <v>23</v>
@@ -1644,10 +1789,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CA33965A-B397-8D4D-8C68-B0CC4C6D2983}">
-  <dimension ref="A1:B6"/>
+  <dimension ref="A1:B7"/>
   <sheetViews>
-    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView topLeftCell="A7" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1669,8 +1814,8 @@
         <v>16</v>
       </c>
       <c r="B2" t="str">
-        <f>"**""" &amp;"&lt;Template_Fraudulent_Activities&gt;"&amp; 'ADCC-Params'!B2&amp; "&lt;/Template_Fraudulent_Activities&gt;"&amp; """**"</f>
-        <v>**"&lt;Template_Fraudulent_Activities&gt;Investment Fraud&lt;/Template_Fraudulent_Activities&gt;"**</v>
+        <f>"**""" &amp;"&lt;Template_FraudulentActivities&gt;"&amp; 'ADCC-Params'!B2&amp; "&lt;/Template_FraudulentActivities&gt;"&amp; """**"</f>
+        <v>**"&lt;Template_FraudulentActivities&gt;Investment Fraud&lt;/Template_FraudulentActivities&gt;"**</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -1682,7 +1827,7 @@
         <v>**[]**</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="94.5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" ht="110.25" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>27</v>
       </c>
@@ -1698,10 +1843,10 @@
 )</f>
         <v>i) The latest balance of the beneficiary account(s);
 ii) Whether the beneficiary account(s) has been suspended after your review. If yes, what functions are blocked;
-iii) The details of next layer beneficiary account(s) relating to the below transaction of [AC1] (including details of transaction, bank, account number and beneficiary name). If the beneficiary account(s) belong to your bank, please provide us the account balance.</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" ht="63" x14ac:dyDescent="0.25">
+iii) The details of next layer beneficiary account(s) relating to the below transaction of [AC1, AC2] (including details of transaction, bank, account number and beneficiary name). If the beneficiary account(s) belong to your bank, please provide us the account balance.</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" ht="170.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>36</v>
       </c>
@@ -1712,12 +1857,21 @@
   _xlpm.tableData, 'ADCC-Beneficiary-Details'!A2:'ADCC-Beneficiary-Details'!E21,
   _xlpm.data, _xlfn._xlws.FILTER(_xlpm.tableData, LEN(INDEX(_xlpm.tableData, 0, 1)) &gt; 0),
   _xlpm.processAcctName, _xlfn.LAMBDA(_xlpm.x, TRIM(SUBSTITUTE(SUBSTITUTE(_xlpm.x, CHAR(10), "&lt;br /&gt;"), """", ""))),
+  _xlpm.Fcol, 'ADCC-Beneficiary-Details'!F2:F21,
   _xlpm.dataProcessed, _xlfn.HSTACK(
-      INDEX(_xlpm.data, , 1),
-      INDEX(_xlpm.data, , 2),
-      INDEX(_xlpm.data, , 3),
-      INDEX(_xlpm.data, , 4),
-      _xlfn.MAP(INDEX(_xlpm.data, , 5), _xlpm.processAcctName)
+    INDEX(_xlpm.data, , 1),
+    _xlfn.MAP(_xlfn.SEQUENCE(ROWS(_xlpm.data)), _xlfn.LAMBDA(_xlpm.i,
+      "&lt;Template_Suspect"&amp;INDEX(_xlpm.Fcol, _xlpm.i)&amp;"_Bank&gt;"&amp;INDEX(_xlpm.data, _xlpm.i, 2)&amp;"&lt;/Template_Suspect"&amp;INDEX(_xlpm.Fcol, _xlpm.i)&amp;"_Bank&gt;"
+    )),
+    INDEX(_xlpm.data, , 3),
+    _xlfn.MAP(_xlfn.SEQUENCE(ROWS(_xlpm.data)), _xlfn.LAMBDA(_xlpm.i,
+      "&lt;Template_Suspect"&amp;INDEX(_xlpm.Fcol, _xlpm.i)&amp;"_AccountNumber&gt;"&amp;INDEX(_xlpm.data, _xlpm.i, 4)&amp;"&lt;/Template_Suspect"&amp;INDEX(_xlpm.Fcol, _xlpm.i)&amp;"_AccountNumber&gt;"
+    )),
+    _xlfn.MAP(_xlfn.SEQUENCE(ROWS(_xlpm.data)), _xlfn.LAMBDA(_xlpm.i,
+      "&lt;Template_Suspect" &amp; INDEX(_xlpm.Fcol, _xlpm.i) &amp; "_Name&gt;" &amp;
+      _xlpm.processAcctName(INDEX(_xlpm.data, _xlpm.i, 5)) &amp;
+      "&lt;/Template_Suspect" &amp; INDEX(_xlpm.Fcol, _xlpm.i) &amp; "_Name&gt;"
+    ))
   ),
   _xlpm.headerRow, "| " &amp; _xlfn.TEXTJOIN(" | ", TRUE, _xlpm.headers) &amp; " |",
   _xlpm.dashRow, "| " &amp; _xlfn.TEXTJOIN(" | ", TRUE, _xlfn.MAP(_xlpm.headers, _xlfn.LAMBDA(_xlpm.x, REPT("-", LEN(_xlpm.x))))) &amp; " |",
@@ -1730,7 +1884,8 @@
 )</f>
         <v>| Ref. | Beneficiary Bank | Layer | Beneficiary Account No. | Beneficiary Account Name |
 | ---- | ---------------- | ----- | ----------------------- | ------------------------ |
-| AC1 | HSB | 1st | 111-111111-101  | CHAN TAI MAN |</v>
+| AC1 | &lt;Template_Suspect1_Bank&gt;HSB&lt;/Template_Suspect1_Bank&gt; | 1st | &lt;Template_Suspect1_AccountNumber&gt;111-111111-101 &lt;/Template_Suspect1_AccountNumber&gt; | &lt;Template_Suspect1_Name&gt;CHAN TAI MAN&lt;/Template_Suspect1_Name&gt; |
+| AC2 | &lt;Template_Suspect2_Bank&gt;HSB&lt;/Template_Suspect2_Bank&gt; | 1st | &lt;Template_Suspect2_AccountNumber&gt;111-111111-102 &lt;/Template_Suspect2_AccountNumber&gt; | &lt;Template_Suspect2_Name&gt;CHUNG SIU&lt;/Template_Suspect2_Name&gt; |</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="307.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -1743,16 +1898,33 @@
   _xlpm.headers, INDEX(_xlpm.rng, 1, _xlfn.SEQUENCE(1, COLUMNS(_xlpm.rng))),
   _xlpm.tableData, 'ADCC-Txn-Details'!A2:'ADCC-Txn-Details'!I21,
   _xlpm.data, _xlfn._xlws.FILTER(_xlpm.tableData, LEN(INDEX(_xlpm.tableData, 0, 1)) &gt; 0),
+  _xlpm.Jcol, 'ADCC-Txn-Details'!J2:J21,
+  _xlpm.Lcol, 'ADCC-Txn-Details'!M2:M21,
+  _xlpm.Mcol, 'ADCC-Txn-Details'!N2:N21,
   _xlpm.dataProcessed, _xlfn.HSTACK(
       INDEX(_xlpm.data, , 1),
-      INDEX(_xlpm.data, , 2),
-      INDEX(_xlpm.data, , 3),
-      INDEX(_xlpm.data, , 4),
-      INDEX(_xlpm.data, , 5),
-      INDEX(_xlpm.data, , 6),
+      _xlfn.MAP(_xlfn.SEQUENCE(ROWS(_xlpm.data)), _xlfn.LAMBDA(_xlpm.i,
+        "&lt;Template_FraudPayment"&amp;INDEX(_xlpm.Jcol, _xlpm.i)&amp;"_Date&gt;"&amp;INDEX(_xlpm.data, _xlpm.i, 2)&amp;"&lt;/Template_FraudPayment"&amp;INDEX(_xlpm.Jcol, _xlpm.i)&amp;"_Date&gt;"
+      )),
+      _xlfn.MAP(_xlfn.SEQUENCE(ROWS(_xlpm.data)), _xlfn.LAMBDA(_xlpm.i,
+        "&lt;Template_FraudPayment"&amp;INDEX(_xlpm.Jcol, _xlpm.i)&amp;"_Currency&gt;"&amp;INDEX(_xlpm.data, _xlpm.i, 3)&amp;"&lt;/Template_FraudPayment"&amp;INDEX(_xlpm.Jcol, _xlpm.i)&amp;"_Currency&gt;"
+      )),
+      _xlfn.MAP(_xlfn.SEQUENCE(ROWS(_xlpm.data)), _xlfn.LAMBDA(_xlpm.i,
+        "&lt;Template_FraudPayment"&amp;INDEX(_xlpm.Jcol, _xlpm.i)&amp;"_Amount&gt;"&amp;INDEX(_xlpm.data, _xlpm.i, 4)&amp;"&lt;/Template_FraudPayment"&amp;INDEX(_xlpm.Jcol, _xlpm.i)&amp;"_Amount&gt;"
+      )),
+      _xlfn.MAP(_xlfn.SEQUENCE(ROWS(_xlpm.data)), _xlfn.LAMBDA(_xlpm.i,
+        "&lt;Template_FraudPayment"&amp;INDEX(_xlpm.Jcol, _xlpm.i)&amp;"_Amount&gt;"&amp;INDEX(_xlpm.data, _xlpm.i, 5)&amp;"&lt;/Template_FraudPayment"&amp;INDEX(_xlpm.Jcol, _xlpm.i)&amp;"_Amount&gt;"
+      )),
+      _xlfn.MAP(_xlfn.SEQUENCE(ROWS(_xlpm.data)), _xlfn.LAMBDA(_xlpm.i,
+        "&lt;Template_Victim"&amp;INDEX(_xlpm.Lcol, _xlpm.i)&amp;"_Account"&amp;INDEX(_xlpm.Mcol, _xlpm.i)&amp;"_Bank&gt;"&amp;INDEX(_xlpm.data, _xlpm.i, 6)&amp;"&lt;/Template_Victim"&amp;INDEX(_xlpm.Lcol, _xlpm.i)&amp;"_Account"&amp;INDEX(_xlpm.Mcol, _xlpm.i)&amp;"_Bank&gt;"
+      )),
       INDEX(_xlpm.data, , 7),
-      INDEX(_xlpm.data, , 8),
-      INDEX(_xlpm.data, , 9)
+      _xlfn.MAP(_xlfn.SEQUENCE(ROWS(_xlpm.data)), _xlfn.LAMBDA(_xlpm.i,
+        "&lt;Template_Victim"&amp;INDEX(_xlpm.Lcol, _xlpm.i)&amp;"_Account"&amp;INDEX(_xlpm.Mcol, _xlpm.i)&amp;"_AccountNumber&gt;"&amp;INDEX(_xlpm.data, _xlpm.i, 8)&amp;"&lt;/Template_Victim"&amp;INDEX(_xlpm.Lcol, _xlpm.i)&amp;"_Account"&amp;INDEX(_xlpm.Mcol, _xlpm.i)&amp;"_AccountNumber&gt;"
+      )),
+      _xlfn.MAP(_xlfn.SEQUENCE(ROWS(_xlpm.data)), _xlfn.LAMBDA(_xlpm.i,
+        "&lt;Template_Victim"&amp;INDEX(_xlpm.Lcol, _xlpm.i)&amp;"_Name&gt;"&amp;INDEX(_xlpm.data, _xlpm.i, 9)&amp;"&lt;/Template_Victim"&amp;INDEX(_xlpm.Lcol, _xlpm.i)&amp;"_Name&gt;"
+      ))
   ),
   _xlpm.headerRow, "| " &amp; _xlfn.TEXTJOIN(" | ", TRUE, _xlpm.headers) &amp; " |",
   _xlpm.dashRow, "| " &amp; _xlfn.TEXTJOIN(" | ", TRUE, _xlfn.MAP(_xlpm.headers, _xlfn.LAMBDA(_xlpm.x, REPT("-", LEN(_xlpm.x))))) &amp; " |",
@@ -1765,18 +1937,157 @@
 )</f>
         <v>| S/N | Date | Currency | Involved Amounts | Approx. HKD | Remitting Bank | AC Location | Depositor AC No. | Depositor AC Name |
 | --- | ---- | -------- | ---------------- | ----------- | -------------- | ----------- | ---------------- | ----------------- |
-| 1 | 2024-08-24 | HKD | 50000 | 50000 | HSBC | Hong Kong | 444-4444444-101 | CHEUNG TAK SHING  |
-| 2 | 2024-08-25 | HKD | 10000 | 10000 | HSBC | Hong Kong | 444-4444444-101 | CHEUNG TAK SHING  |
-| 1 | 2024-08-24 | HKD | 31000 | 31000 | HSB | Hong Kong | 222-222222-101  | CHEUNG TAK SHING  |
-| 2 | 2024-08-25 | HKD | 50000 | 50000 | HSB | Hong Kong | 222-222222-101  | CHEUNG TAK SHING  |
-| 3 | 2024-08-25 | HKD | 60000 | 60000 | HSB | Hong Kong | 222-222222-101  | CHEUNG TAK SHING  |
-| 4 | 2024-08-25 | HKD | 30000 | 30000 | HSB | Hong Kong | 222-222222-101  | CHEUNG TAK SHING  |
-| 1 | 2024-08-25 | HKD | 39000 | 39000 | Hong Kong | CHEUNG TAK SHING  |</v>
+| 1 | &lt;Template_FraudPayment2_Date&gt;2024-08-24&lt;/Template_FraudPayment2_Date&gt; | &lt;Template_FraudPayment2_Currency&gt;HKD&lt;/Template_FraudPayment2_Currency&gt; | &lt;Template_FraudPayment2_Amount&gt;50000&lt;/Template_FraudPayment2_Amount&gt; | &lt;Template_FraudPayment2_Amount&gt;50000&lt;/Template_FraudPayment2_Amount&gt; | &lt;Template_Victim1_Account1_Bank&gt;HSBC&lt;/Template_Victim1_Account1_Bank&gt; | Hong Kong | &lt;Template_Victim1_Account1_AccountNumber&gt;444-4444444-101&lt;/Template_Victim1_Account1_AccountNumber&gt; | &lt;Template_Victim1_Name&gt;CHEUNG TAK SHING &lt;/Template_Victim1_Name&gt; |
+| 2 | &lt;Template_FraudPayment3_Date&gt;2024-08-25&lt;/Template_FraudPayment3_Date&gt; | &lt;Template_FraudPayment3_Currency&gt;HKD&lt;/Template_FraudPayment3_Currency&gt; | &lt;Template_FraudPayment3_Amount&gt;10000&lt;/Template_FraudPayment3_Amount&gt; | &lt;Template_FraudPayment3_Amount&gt;10000&lt;/Template_FraudPayment3_Amount&gt; | &lt;Template_Victim1_Account1_Bank&gt;HSBC&lt;/Template_Victim1_Account1_Bank&gt; | Hong Kong | &lt;Template_Victim1_Account1_AccountNumber&gt;444-4444444-101&lt;/Template_Victim1_Account1_AccountNumber&gt; | &lt;Template_Victim1_Name&gt;CHEUNG TAK SHING &lt;/Template_Victim1_Name&gt; |
+| 1 | &lt;Template_FraudPayment4_Date&gt;2024-08-24&lt;/Template_FraudPayment4_Date&gt; | &lt;Template_FraudPayment4_Currency&gt;HKD&lt;/Template_FraudPayment4_Currency&gt; | &lt;Template_FraudPayment4_Amount&gt;31000&lt;/Template_FraudPayment4_Amount&gt; | &lt;Template_FraudPayment4_Amount&gt;31000&lt;/Template_FraudPayment4_Amount&gt; | &lt;Template_Victim1_Account2_Bank&gt;HSB&lt;/Template_Victim1_Account2_Bank&gt; | Hong Kong | &lt;Template_Victim1_Account2_AccountNumber&gt;222-222222-101 &lt;/Template_Victim1_Account2_AccountNumber&gt; | &lt;Template_Victim1_Name&gt;CHEUNG TAK SHING &lt;/Template_Victim1_Name&gt; |
+| 2 | &lt;Template_FraudPayment5_Date&gt;2024-08-25&lt;/Template_FraudPayment5_Date&gt; | &lt;Template_FraudPayment5_Currency&gt;HKD&lt;/Template_FraudPayment5_Currency&gt; | &lt;Template_FraudPayment5_Amount&gt;50000&lt;/Template_FraudPayment5_Amount&gt; | &lt;Template_FraudPayment5_Amount&gt;50000&lt;/Template_FraudPayment5_Amount&gt; | &lt;Template_Victim1_Account2_Bank&gt;HSB&lt;/Template_Victim1_Account2_Bank&gt; | Hong Kong | &lt;Template_Victim1_Account2_AccountNumber&gt;222-222222-101 &lt;/Template_Victim1_Account2_AccountNumber&gt; | &lt;Template_Victim1_Name&gt;CHEUNG TAK SHING &lt;/Template_Victim1_Name&gt; |
+| 3 | &lt;Template_FraudPayment6_Date&gt;2024-08-25&lt;/Template_FraudPayment6_Date&gt; | &lt;Template_FraudPayment6_Currency&gt;HKD&lt;/Template_FraudPayment6_Currency&gt; | &lt;Template_FraudPayment6_Amount&gt;60000&lt;/Template_FraudPayment6_Amount&gt; | &lt;Template_FraudPayment6_Amount&gt;60000&lt;/Template_FraudPayment6_Amount&gt; | &lt;Template_Victim1_Account2_Bank&gt;HSB&lt;/Template_Victim1_Account2_Bank&gt; | Hong Kong | &lt;Template_Victim1_Account2_AccountNumber&gt;222-222222-101 &lt;/Template_Victim1_Account2_AccountNumber&gt; | &lt;Template_Victim1_Name&gt;CHEUNG TAK SHING &lt;/Template_Victim1_Name&gt; |
+| 4 | &lt;Template_FraudPayment7_Date&gt;2024-08-25&lt;/Template_FraudPayment7_Date&gt; | &lt;Template_FraudPayment7_Currency&gt;HKD&lt;/Template_FraudPayment7_Currency&gt; | &lt;Template_FraudPayment7_Amount&gt;30000&lt;/Template_FraudPayment7_Amount&gt; | &lt;Template_FraudPayment7_Amount&gt;30000&lt;/Template_FraudPayment7_Amount&gt; | &lt;Template_Victim1_Account2_Bank&gt;HSB&lt;/Template_Victim1_Account2_Bank&gt; | Hong Kong | &lt;Template_Victim1_Account2_AccountNumber&gt;222-222222-101 &lt;/Template_Victim1_Account2_AccountNumber&gt; | &lt;Template_Victim1_Name&gt;CHEUNG TAK SHING &lt;/Template_Victim1_Name&gt; |
+| 1 | &lt;Template_FraudPayment8_Date&gt;2024-08-25&lt;/Template_FraudPayment8_Date&gt; | &lt;Template_FraudPayment8_Currency&gt;HKD&lt;/Template_FraudPayment8_Currency&gt; | &lt;Template_FraudPayment8_Amount&gt;39000&lt;/Template_FraudPayment8_Amount&gt; | &lt;Template_FraudPayment8_Amount&gt;39000&lt;/Template_FraudPayment8_Amount&gt; | &lt;Template_Victim1_Account3_Bank&gt;&lt;/Template_Victim1_Account3_Bank&gt; | Hong Kong | &lt;Template_Victim1_Account3_AccountNumber&gt;&lt;/Template_Victim1_Account3_AccountNumber&gt; | &lt;Template_Victim1_Name&gt;CHEUNG TAK SHING &lt;/Template_Victim1_Name&gt; |
+| 1 | &lt;Template_FraudPayment9_Date&gt;2024-08-25&lt;/Template_FraudPayment9_Date&gt; | &lt;Template_FraudPayment9_Currency&gt;HKD&lt;/Template_FraudPayment9_Currency&gt; | &lt;Template_FraudPayment9_Amount&gt;50000&lt;/Template_FraudPayment9_Amount&gt; | &lt;Template_FraudPayment9_Amount&gt;50000&lt;/Template_FraudPayment9_Amount&gt; | &lt;Template_Victim1_Account1_Bank&gt;HSBC&lt;/Template_Victim1_Account1_Bank&gt; | Hong Kong | &lt;Template_Victim1_Account1_AccountNumber&gt;444-4444444-101&lt;/Template_Victim1_Account1_AccountNumber&gt; | &lt;Template_Victim1_Name&gt;CHEUNG TAK SHING &lt;/Template_Victim1_Name&gt; |
+| 1 | &lt;Template_FraudPayment10_Date&gt;2024-08-25&lt;/Template_FraudPayment10_Date&gt; | &lt;Template_FraudPayment10_Currency&gt;HKD&lt;/Template_FraudPayment10_Currency&gt; | &lt;Template_FraudPayment10_Amount&gt;50000&lt;/Template_FraudPayment10_Amount&gt; | &lt;Template_FraudPayment10_Amount&gt;50000&lt;/Template_FraudPayment10_Amount&gt; | &lt;Template_Victim1_Account2_Bank&gt;HSB&lt;/Template_Victim1_Account2_Bank&gt; | Hong Kong | &lt;Template_Victim1_Account2_AccountNumber&gt;222-222222-101 &lt;/Template_Victim1_Account2_AccountNumber&gt; | &lt;Template_Victim1_Name&gt;CHEUNG TAK SHING &lt;/Template_Victim1_Name&gt; |</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" ht="409.5" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>111</v>
+      </c>
+      <c r="B7" s="1" t="str" cm="1">
+        <f t="array" ref="B7">_xlfn.LET(
+  _xlpm.benRng, 'ADCC-Beneficiary-Details'!A1:E21,
+  _xlpm.benHeaders, INDEX(_xlpm.benRng, 1, _xlfn.SEQUENCE(1, COLUMNS(_xlpm.benRng))),
+  _xlpm.benTableData, 'ADCC-Beneficiary-Details'!A2:E21,
+  _xlpm.benData, _xlfn._xlws.FILTER(_xlpm.benTableData, LEN(INDEX(_xlpm.benTableData, 0, 1)) &gt; 0),
+  _xlpm.benFcol, _xlfn._xlws.FILTER('ADCC-Beneficiary-Details'!F2:F21, LEN(INDEX(_xlpm.benTableData, 0, 1)) &gt; 0),
+  _xlpm.processAcctName, _xlfn.LAMBDA(_xlpm.x, TRIM(SUBSTITUTE(SUBSTITUTE(_xlpm.x, CHAR(10), "&lt;br /&gt;"), """", ""))),
+  _xlpm.txnRng, 'ADCC-Txn-Details'!A1:I21,
+  _xlpm.txnHeaders, INDEX(_xlpm.txnRng, 1, _xlfn.SEQUENCE(1, COLUMNS(_xlpm.txnRng))),
+  _xlpm.txnTableData, 'ADCC-Txn-Details'!A2:I21,
+  _xlpm.txnJcol, 'ADCC-Txn-Details'!J2:J21,
+  _xlpm.txnLcol, 'ADCC-Txn-Details'!L2:L21,
+  _xlpm.txnMcol, 'ADCC-Txn-Details'!M2:M21,
+  _xlpm.txnNcol, 'ADCC-Txn-Details'!N2:N21,
+  _xlpm.groups, _xlfn.UNIQUE(_xlfn._xlws.FILTER(_xlpm.benFcol, _xlpm.benFcol&lt;&gt;"")),
+  _xlpm.makeSection, _xlfn.LAMBDA(_xlpm.group,
+    _xlfn.LET(
+      _xlpm.benRowIndices, _xlfn._xlws.FILTER(_xlfn.SEQUENCE(ROWS(_xlpm.benFcol)), _xlpm.benFcol=_xlpm.group),
+      _xlpm.benRows, INDEX(_xlpm.benData, _xlpm.benRowIndices, _xlfn.SEQUENCE(1, COLUMNS(_xlpm.benData))),
+      _xlpm.benProcessed, _xlfn.HSTACK(
+        INDEX(_xlpm.benRows, , 1),
+        _xlfn.MAP(_xlfn.SEQUENCE(ROWS(_xlpm.benRows)), _xlfn.LAMBDA(_xlpm.i,
+          "&lt;Template_Suspect_"&amp;_xlpm.group&amp;"_Bank&gt;"&amp;INDEX(_xlpm.benRows, _xlpm.i, 2)&amp;"&lt;/Template_Suspect_"&amp;_xlpm.group&amp;"_Bank&gt;"
+        )),
+        INDEX(_xlpm.benRows, , 3),
+        _xlfn.MAP(_xlfn.SEQUENCE(ROWS(_xlpm.benRows)), _xlfn.LAMBDA(_xlpm.i,
+          "&lt;Template_Suspect_"&amp;_xlpm.group&amp;"_Account_Number&gt;"&amp;INDEX(_xlpm.benRows, _xlpm.i, 4)&amp;"&lt;/Template_Suspect_"&amp;_xlpm.group&amp;"_Account_Number&gt;"
+        )),
+        _xlfn.MAP(_xlfn.SEQUENCE(ROWS(_xlpm.benRows)), _xlfn.LAMBDA(_xlpm.i,
+          "&lt;Template_Suspect_" &amp; _xlpm.group &amp; "_Name&gt;" &amp;
+          _xlpm.processAcctName(INDEX(_xlpm.benRows, _xlpm.i, 5)) &amp;
+          "&lt;/Template_Suspect_" &amp; _xlpm.group &amp; "_Name&gt;"
+        ))
+      ),
+      _xlpm.benHeaderRow, "| " &amp; _xlfn.TEXTJOIN(" | ", TRUE, _xlpm.benHeaders) &amp; " |",
+      _xlpm.benDashRow, "| " &amp; _xlfn.TEXTJOIN(" | ", TRUE, _xlfn.MAP(_xlpm.benHeaders, _xlfn.LAMBDA(_xlpm.x, REPT("-", LEN(_xlpm.x))))) &amp; " |",
+      _xlpm.benDataRows, _xlfn.TEXTJOIN(CHAR(10), TRUE,
+        _xlfn.MAP(_xlfn.SEQUENCE(ROWS(_xlpm.benProcessed)), _xlfn.LAMBDA(_xlpm.i,
+          "| " &amp; _xlfn.TEXTJOIN(" | ", TRUE, INDEX(_xlpm.benProcessed, _xlpm.i, )) &amp; " |"
+        ))
+      ),
+      _xlpm.benTable, "Details of Beneficiary" &amp; CHAR(10) &amp; _xlpm.benHeaderRow &amp; CHAR(10) &amp; _xlpm.benDashRow &amp; CHAR(10) &amp; _xlpm.benDataRows,
+      _xlpm.txnForGroup, _xlfn._xlws.FILTER(_xlpm.txnTableData, _xlpm.txnLcol=_xlpm.group),
+      _xlpm.txnJForGroup, _xlfn._xlws.FILTER(_xlpm.txnJcol, _xlpm.txnLcol=_xlpm.group),
+      _xlpm.txnMForGroup, _xlfn._xlws.FILTER(_xlpm.txnMcol, _xlpm.txnLcol=_xlpm.group),
+      _xlpm.txnNForGroup, _xlfn._xlws.FILTER(_xlpm.txnNcol, _xlpm.txnLcol=_xlpm.group),
+      _xlpm.mnCombined, _xlpm.txnMForGroup &amp; "-" &amp; _xlpm.txnNForGroup,
+      _xlpm.txnSubGroups, _xlfn.UNIQUE(_xlfn._xlws.FILTER(_xlpm.mnCombined, _xlpm.mnCombined&lt;&gt;"")),
+      _xlpm.makeTxnTable, _xlfn.LAMBDA(_xlpm.subGroup,
+        _xlfn.LET(
+          _xlpm.subIndices, _xlfn._xlws.FILTER(_xlfn.SEQUENCE(ROWS(_xlpm.mnCombined)), _xlpm.mnCombined=_xlpm.subGroup),
+          _xlpm.txnRows, INDEX(_xlpm.txnForGroup, _xlpm.subIndices, _xlfn.SEQUENCE(1, COLUMNS(_xlpm.txnForGroup))),
+          _xlpm.subJcol, INDEX(_xlpm.txnJForGroup, _xlpm.subIndices),
+          _xlpm.subMcol, INDEX(_xlpm.txnMForGroup, _xlpm.subIndices),
+          _xlpm.subNcol, INDEX(_xlpm.txnNForGroup, _xlpm.subIndices),
+          _xlpm.txnProcessed, _xlfn.HSTACK(
+            INDEX(_xlpm.txnRows, , 1),
+            _xlfn.MAP(_xlfn.SEQUENCE(ROWS(_xlpm.txnRows)), _xlfn.LAMBDA(_xlpm.i,
+              "&lt;Template_FraudPayment"&amp;INDEX(_xlpm.subJcol, _xlpm.i)&amp;"_Date&gt;"&amp;INDEX(_xlpm.txnRows, _xlpm.i, 2)&amp;"&lt;/Template_FraudPayment"&amp;INDEX(_xlpm.subJcol, _xlpm.i)&amp;"_Date&gt;"
+            )),
+            _xlfn.MAP(_xlfn.SEQUENCE(ROWS(_xlpm.txnRows)), _xlfn.LAMBDA(_xlpm.i,
+              "&lt;Template_FraudPayment"&amp;INDEX(_xlpm.subJcol, _xlpm.i)&amp;"_Currency&gt;"&amp;INDEX(_xlpm.txnRows, _xlpm.i, 3)&amp;"&lt;/Template_FraudPayment"&amp;INDEX(_xlpm.subJcol, _xlpm.i)&amp;"_Currency&gt;"
+            )),
+            _xlfn.MAP(_xlfn.SEQUENCE(ROWS(_xlpm.txnRows)), _xlfn.LAMBDA(_xlpm.i,
+              "&lt;Template_FraudPayment"&amp;INDEX(_xlpm.subJcol, _xlpm.i)&amp;"_Amount&gt;"&amp;INDEX(_xlpm.txnRows, _xlpm.i, 4)&amp;"&lt;/Template_FraudPayment"&amp;INDEX(_xlpm.subJcol, _xlpm.i)&amp;"_Amount&gt;"
+            )),
+            _xlfn.MAP(_xlfn.SEQUENCE(ROWS(_xlpm.txnRows)), _xlfn.LAMBDA(_xlpm.i,
+              "&lt;Template_FraudPayment"&amp;INDEX(_xlpm.subJcol, _xlpm.i)&amp;"_Amount&gt;"&amp;INDEX(_xlpm.txnRows, _xlpm.i, 5)&amp;"&lt;/Template_FraudPayment"&amp;INDEX(_xlpm.subJcol, _xlpm.i)&amp;"_Amount&gt;"
+            )),
+            _xlfn.MAP(_xlfn.SEQUENCE(ROWS(_xlpm.txnRows)), _xlfn.LAMBDA(_xlpm.i,
+              "&lt;Template_Victim"&amp;INDEX(_xlpm.subMcol, _xlpm.i)&amp;"_Account"&amp;INDEX(_xlpm.subNcol, _xlpm.i)&amp;"_Bank&gt;"&amp;INDEX(_xlpm.txnRows, _xlpm.i, 6)&amp;"&lt;/Template_Victim"&amp;INDEX(_xlpm.subMcol, _xlpm.i)&amp;"_Account"&amp;INDEX(_xlpm.subNcol, _xlpm.i)&amp;"_Bank&gt;"
+            )),
+            INDEX(_xlpm.txnRows, , 7),
+            _xlfn.MAP(_xlfn.SEQUENCE(ROWS(_xlpm.txnRows)), _xlfn.LAMBDA(_xlpm.i,
+              "&lt;Template_Victim"&amp;INDEX(_xlpm.subMcol, _xlpm.i)&amp;"_Account"&amp;INDEX(_xlpm.subNcol, _xlpm.i)&amp;"_AccountNumber&gt;"&amp;INDEX(_xlpm.txnRows, _xlpm.i, 8)&amp;"&lt;/Template_Victim"&amp;INDEX(_xlpm.subMcol, _xlpm.i)&amp;"_Account"&amp;INDEX(_xlpm.subNcol, _xlpm.i)&amp;"_AccountNumber&gt;"
+            )),
+            _xlfn.MAP(_xlfn.SEQUENCE(ROWS(_xlpm.txnRows)), _xlfn.LAMBDA(_xlpm.i,
+              "&lt;Template_Victim"&amp;INDEX(_xlpm.subMcol, _xlpm.i)&amp;"_Name&gt;"&amp;INDEX(_xlpm.txnRows, _xlpm.i, 9)&amp;"&lt;/Template_Victim"&amp;INDEX(_xlpm.subMcol, _xlpm.i)&amp;"_Name&gt;"
+            ))
+          ),
+          _xlpm.txnHeaderRow, "| " &amp; _xlfn.TEXTJOIN(" | ", TRUE, _xlpm.txnHeaders) &amp; " |",
+          _xlpm.txnDashRow, "| " &amp; _xlfn.TEXTJOIN(" | ", TRUE, _xlfn.MAP(_xlpm.txnHeaders, _xlfn.LAMBDA(_xlpm.x, REPT("-", LEN(_xlpm.x))))) &amp; " |",
+          _xlpm.txnDataRows, _xlfn.TEXTJOIN(CHAR(10), TRUE,
+            _xlfn.MAP(_xlfn.SEQUENCE(ROWS(_xlpm.txnProcessed)), _xlfn.LAMBDA(_xlpm.i,
+              "| " &amp; _xlfn.TEXTJOIN(" | ", TRUE, INDEX(_xlpm.txnProcessed, _xlpm.i, )) &amp; " |"
+            ))
+          ),
+          "Transaction Details" &amp; CHAR(10) &amp; _xlpm.txnHeaderRow &amp; CHAR(10) &amp; _xlpm.txnDashRow &amp; CHAR(10) &amp; _xlpm.txnDataRows
+        )
+      ),
+      _xlpm.allTxnTables, _xlfn.TEXTJOIN(CHAR(10) &amp; CHAR(10), TRUE, _xlfn.MAP(_xlpm.txnSubGroups, _xlpm.makeTxnTable)),
+      _xlpm.benTable &amp; CHAR(10) &amp; CHAR(10) &amp; _xlpm.allTxnTables &amp; CHAR(10) &amp; CHAR(10) &amp; IF('ADCC-Params'!B6="Y","\*\*STR\*\*","\*\*NO STR\*\*")
+    )
+  ),
+  _xlfn.TEXTJOIN(CHAR(10) &amp; CHAR(10), TRUE, _xlfn.MAP(_xlpm.groups, _xlpm.makeSection))
+)</f>
+        <v>Details of Beneficiary
+| Ref. | Beneficiary Bank | Layer | Beneficiary Account No. | Beneficiary Account Name |
+| ---- | ---------------- | ----- | ----------------------- | ------------------------ |
+| AC1 | &lt;Template_Suspect_1_Bank&gt;HSB&lt;/Template_Suspect_1_Bank&gt; | 1st | &lt;Template_Suspect_1_Account_Number&gt;111-111111-101 &lt;/Template_Suspect_1_Account_Number&gt; | &lt;Template_Suspect_1_Name&gt;CHAN TAI MAN&lt;/Template_Suspect_1_Name&gt; |
+Transaction Details
+| S/N | Date | Currency | Involved Amounts | Approx. HKD | Remitting Bank | AC Location | Depositor AC No. | Depositor AC Name |
+| --- | ---- | -------- | ---------------- | ----------- | -------------- | ----------- | ---------------- | ----------------- |
+| 1 | &lt;Template_FraudPayment2_Date&gt;2024-08-24&lt;/Template_FraudPayment2_Date&gt; | &lt;Template_FraudPayment2_Currency&gt;HKD&lt;/Template_FraudPayment2_Currency&gt; | &lt;Template_FraudPayment2_Amount&gt;50000&lt;/Template_FraudPayment2_Amount&gt; | &lt;Template_FraudPayment2_Amount&gt;50000&lt;/Template_FraudPayment2_Amount&gt; | &lt;Template_Victim1_Account1_Bank&gt;HSBC&lt;/Template_Victim1_Account1_Bank&gt; | Hong Kong | &lt;Template_Victim1_Account1_AccountNumber&gt;444-4444444-101&lt;/Template_Victim1_Account1_AccountNumber&gt; | &lt;Template_Victim1_Name&gt;CHEUNG TAK SHING &lt;/Template_Victim1_Name&gt; |
+| 2 | &lt;Template_FraudPayment3_Date&gt;2024-08-25&lt;/Template_FraudPayment3_Date&gt; | &lt;Template_FraudPayment3_Currency&gt;HKD&lt;/Template_FraudPayment3_Currency&gt; | &lt;Template_FraudPayment3_Amount&gt;10000&lt;/Template_FraudPayment3_Amount&gt; | &lt;Template_FraudPayment3_Amount&gt;10000&lt;/Template_FraudPayment3_Amount&gt; | &lt;Template_Victim1_Account1_Bank&gt;HSBC&lt;/Template_Victim1_Account1_Bank&gt; | Hong Kong | &lt;Template_Victim1_Account1_AccountNumber&gt;444-4444444-101&lt;/Template_Victim1_Account1_AccountNumber&gt; | &lt;Template_Victim1_Name&gt;CHEUNG TAK SHING &lt;/Template_Victim1_Name&gt; |
+Transaction Details
+| S/N | Date | Currency | Involved Amounts | Approx. HKD | Remitting Bank | AC Location | Depositor AC No. | Depositor AC Name |
+| --- | ---- | -------- | ---------------- | ----------- | -------------- | ----------- | ---------------- | ----------------- |
+| 1 | &lt;Template_FraudPayment4_Date&gt;2024-08-24&lt;/Template_FraudPayment4_Date&gt; | &lt;Template_FraudPayment4_Currency&gt;HKD&lt;/Template_FraudPayment4_Currency&gt; | &lt;Template_FraudPayment4_Amount&gt;31000&lt;/Template_FraudPayment4_Amount&gt; | &lt;Template_FraudPayment4_Amount&gt;31000&lt;/Template_FraudPayment4_Amount&gt; | &lt;Template_Victim1_Account2_Bank&gt;HSB&lt;/Template_Victim1_Account2_Bank&gt; | Hong Kong | &lt;Template_Victim1_Account2_AccountNumber&gt;222-222222-101 &lt;/Template_Victim1_Account2_AccountNumber&gt; | &lt;Template_Victim1_Name&gt;CHEUNG TAK SHING &lt;/Template_Victim1_Name&gt; |
+| 2 | &lt;Template_FraudPayment5_Date&gt;2024-08-25&lt;/Template_FraudPayment5_Date&gt; | &lt;Template_FraudPayment5_Currency&gt;HKD&lt;/Template_FraudPayment5_Currency&gt; | &lt;Template_FraudPayment5_Amount&gt;50000&lt;/Template_FraudPayment5_Amount&gt; | &lt;Template_FraudPayment5_Amount&gt;50000&lt;/Template_FraudPayment5_Amount&gt; | &lt;Template_Victim1_Account2_Bank&gt;HSB&lt;/Template_Victim1_Account2_Bank&gt; | Hong Kong | &lt;Template_Victim1_Account2_AccountNumber&gt;222-222222-101 &lt;/Template_Victim1_Account2_AccountNumber&gt; | &lt;Template_Victim1_Name&gt;CHEUNG TAK SHING &lt;/Template_Victim1_Name&gt; |
+| 3 | &lt;Template_FraudPayment6_Date&gt;2024-08-25&lt;/Template_FraudPayment6_Date&gt; | &lt;Template_FraudPayment6_Currency&gt;HKD&lt;/Template_FraudPayment6_Currency&gt; | &lt;Template_FraudPayment6_Amount&gt;60000&lt;/Template_FraudPayment6_Amount&gt; | &lt;Template_FraudPayment6_Amount&gt;60000&lt;/Template_FraudPayment6_Amount&gt; | &lt;Template_Victim1_Account2_Bank&gt;HSB&lt;/Template_Victim1_Account2_Bank&gt; | Hong Kong | &lt;Template_Victim1_Account2_AccountNumber&gt;222-222222-101 &lt;/Template_Victim1_Account2_AccountNumber&gt; | &lt;Template_Victim1_Name&gt;CHEUNG TAK SHING &lt;/Template_Victim1_Name&gt; |
+| 4 | &lt;Template_FraudPayment7_Date&gt;2024-08-25&lt;/Template_FraudPayment7_Date&gt; | &lt;Template_FraudPayment7_Currency&gt;HKD&lt;/Template_FraudPayment7_Currency&gt; | &lt;Template_FraudPayment7_Amount&gt;30000&lt;/Template_FraudPayment7_Amount&gt; | &lt;Template_FraudPayment7_Amount&gt;30000&lt;/Template_FraudPayment7_Amount&gt; | &lt;Template_Victim1_Account2_Bank&gt;HSB&lt;/Template_Victim1_Account2_Bank&gt; | Hong Kong | &lt;Template_Victim1_Account2_AccountNumber&gt;222-222222-101 &lt;/Template_Victim1_Account2_AccountNumber&gt; | &lt;Template_Victim1_Name&gt;CHEUNG TAK SHING &lt;/Template_Victim1_Name&gt; |
+Transaction Details
+| S/N | Date | Currency | Involved Amounts | Approx. HKD | Remitting Bank | AC Location | Depositor AC No. | Depositor AC Name |
+| --- | ---- | -------- | ---------------- | ----------- | -------------- | ----------- | ---------------- | ----------------- |
+| 1 | &lt;Template_FraudPayment8_Date&gt;2024-08-25&lt;/Template_FraudPayment8_Date&gt; | &lt;Template_FraudPayment8_Currency&gt;HKD&lt;/Template_FraudPayment8_Currency&gt; | &lt;Template_FraudPayment8_Amount&gt;39000&lt;/Template_FraudPayment8_Amount&gt; | &lt;Template_FraudPayment8_Amount&gt;39000&lt;/Template_FraudPayment8_Amount&gt; | &lt;Template_Victim1_Account3_Bank&gt;&lt;/Template_Victim1_Account3_Bank&gt; | Hong Kong | &lt;Template_Victim1_Account3_AccountNumber&gt;&lt;/Template_Victim1_Account3_AccountNumber&gt; | &lt;Template_Victim1_Name&gt;CHEUNG TAK SHING &lt;/Template_Victim1_Name&gt; |
+\*\*NO STR\*\*
+Details of Beneficiary
+| Ref. | Beneficiary Bank | Layer | Beneficiary Account No. | Beneficiary Account Name |
+| ---- | ---------------- | ----- | ----------------------- | ------------------------ |
+| AC2 | &lt;Template_Suspect_2_Bank&gt;HSB&lt;/Template_Suspect_2_Bank&gt; | 1st | &lt;Template_Suspect_2_Account_Number&gt;111-111111-102 &lt;/Template_Suspect_2_Account_Number&gt; | &lt;Template_Suspect_2_Name&gt;CHUNG SIU&lt;/Template_Suspect_2_Name&gt; |
+Transaction Details
+| S/N | Date | Currency | Involved Amounts | Approx. HKD | Remitting Bank | AC Location | Depositor AC No. | Depositor AC Name |
+| --- | ---- | -------- | ---------------- | ----------- | -------------- | ----------- | ---------------- | ----------------- |
+| 1 | &lt;Template_FraudPayment9_Date&gt;2024-08-25&lt;/Template_FraudPayment9_Date&gt; | &lt;Template_FraudPayment9_Currency&gt;HKD&lt;/Template_FraudPayment9_Currency&gt; | &lt;Template_FraudPayment9_Amount&gt;50000&lt;/Template_FraudPayment9_Amount&gt; | &lt;Template_FraudPayment9_Amount&gt;50000&lt;/Template_FraudPayment9_Amount&gt; | &lt;Template_Victim1_Account1_Bank&gt;HSBC&lt;/Template_Victim1_Account1_Bank&gt; | Hong Kong | &lt;Template_Victim1_Account1_AccountNumber&gt;444-4444444-101&lt;/Template_Victim1_Account1_AccountNumber&gt; | &lt;Template_Victim1_Name&gt;CHEUNG TAK SHING &lt;/Template_Victim1_Name&gt; |
+Transaction Details
+| S/N | Date | Currency | Involved Amounts | Approx. HKD | Remitting Bank | AC Location | Depositor AC No. | Depositor AC Name |
+| --- | ---- | -------- | ---------------- | ----------- | -------------- | ----------- | ---------------- | ----------------- |
+| 1 | &lt;Template_FraudPayment10_Date&gt;2024-08-25&lt;/Template_FraudPayment10_Date&gt; | &lt;Template_FraudPayment10_Currency&gt;HKD&lt;/Template_FraudPayment10_Currency&gt; | &lt;Template_FraudPayment10_Amount&gt;50000&lt;/Template_FraudPayment10_Amount&gt; | &lt;Template_FraudPayment10_Amount&gt;50000&lt;/Template_FraudPayment10_Amount&gt; | &lt;Template_Victim1_Account2_Bank&gt;HSB&lt;/Template_Victim1_Account2_Bank&gt; | Hong Kong | &lt;Template_Victim1_Account2_AccountNumber&gt;222-222222-101 &lt;/Template_Victim1_Account2_AccountNumber&gt; | &lt;Template_Victim1_Name&gt;CHEUNG TAK SHING &lt;/Template_Victim1_Name&gt; |
+\*\*NO STR\*\*</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1784,8 +2095,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{20049DAE-7D29-4C48-8C4E-F65336495C09}">
   <dimension ref="A1:B21"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+    <sheetView topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1970,10 +2281,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{21DA51B1-9D3A-004F-B268-14C997F191DB}">
-  <dimension ref="A1:A28"/>
+  <dimension ref="A1:A23"/>
   <sheetViews>
-    <sheetView zoomScale="90" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+    <sheetView topLeftCell="A3" zoomScale="90" workbookViewId="0">
+      <selection activeCell="A7" sqref="A7:XFD7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1987,10 +2298,10 @@
         <v>Dear HSB,</v>
       </c>
     </row>
-    <row r="3" spans="1:1" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:1" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="str">
-        <f>'ADCC-Template'!B3&amp;'ADCC-Runtime-Params'!B2&amp;'ADCC-Template'!B4&amp;"**"&amp;'ADCC-Params'!B3&amp;"**"&amp;'ADCC-Template'!B5&amp;"**"&amp;"&lt;Template_Police_Investigation_Team_Name&gt;"&amp;'ADCC-Params'!B4&amp;"&lt;/Template_Police_Investigation_Team_Name&gt;"&amp;"**"&amp;'ADCC-Template'!B6&amp;'ADCC-Runtime-Params'!B3</f>
-        <v>Please be informed of a case of **"&lt;Template_Fraudulent_Activities&gt;Investment Fraud&lt;/Template_Fraudulent_Activities&gt;"** reported on **2024-09-01** and it is under the investigation by **&lt;Template_Police_Investigation_Team_Name&gt;DIT2-■■■■■&lt;/Template_Police_Investigation_Team_Name&gt;**. It is alleged that the relevant crime proceeds were transferred to the account(s) below **[]**</v>
+        <f>'ADCC-Template'!B3&amp;'ADCC-Runtime-Params'!B2&amp;'ADCC-Template'!B4&amp;"**"&amp;'ADCC-Params'!B3&amp;"**"&amp;'ADCC-Template'!B5&amp;"**"&amp;"&lt;Template_PoliceInvestigationTeamName&gt;"&amp;'ADCC-Params'!B4&amp;"&lt;/Template_PoliceInvestigationTeamName&gt;"&amp;"**"&amp;'ADCC-Template'!B6&amp;'ADCC-Runtime-Params'!B3</f>
+        <v>Please be informed of a case of **"&lt;Template_FraudulentActivities&gt;Investment Fraud&lt;/Template_FraudulentActivities&gt;"** reported on **2024-09-01** and it is under the investigation by **&lt;Template_PoliceInvestigationTeamName&gt;DIT2-■■■■■&lt;/Template_PoliceInvestigationTeamName&gt;**. It is alleged that the relevant crime proceeds were transferred to the account(s) below **[]**</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.25">
@@ -2004,107 +2315,103 @@
         <f>'ADCC-Runtime-Params'!B4</f>
         <v>i) The latest balance of the beneficiary account(s);
 ii) Whether the beneficiary account(s) has been suspended after your review. If yes, what functions are blocked;
-iii) The details of next layer beneficiary account(s) relating to the below transaction of [AC1] (including details of transaction, bank, account number and beneficiary name). If the beneficiary account(s) belong to your bank, please provide us the account balance.</v>
+iii) The details of next layer beneficiary account(s) relating to the below transaction of [AC1, AC2] (including details of transaction, bank, account number and beneficiary name). If the beneficiary account(s) belong to your bank, please provide us the account balance.</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7" s="1" t="str">
-        <f>'ADCC-Template'!B8</f>
-        <v>Details of Beneficiary</v>
-      </c>
-    </row>
-    <row r="8" spans="1:1" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="A7" s="1"/>
+    </row>
+    <row r="8" spans="1:1" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="str">
-        <f>'ADCC-Runtime-Params'!B5</f>
-        <v>| Ref. | Beneficiary Bank | Layer | Beneficiary Account No. | Beneficiary Account Name |
+        <f>'ADCC-Runtime-Params'!B7</f>
+        <v>Details of Beneficiary
+| Ref. | Beneficiary Bank | Layer | Beneficiary Account No. | Beneficiary Account Name |
 | ---- | ---------------- | ----- | ----------------------- | ------------------------ |
-| AC1 | HSB | 1st | 111-111111-101  | CHAN TAI MAN |</v>
-      </c>
-    </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A9" s="1"/>
-    </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A10" t="str">
-        <f>'ADCC-Template'!B9</f>
-        <v>Transaction Details</v>
-      </c>
-    </row>
-    <row r="11" spans="1:1" ht="63" x14ac:dyDescent="0.25">
-      <c r="A11" s="1" t="str">
-        <f>'ADCC-Runtime-Params'!B6</f>
-        <v>| S/N | Date | Currency | Involved Amounts | Approx. HKD | Remitting Bank | AC Location | Depositor AC No. | Depositor AC Name |
+| AC1 | &lt;Template_Suspect_1_Bank&gt;HSB&lt;/Template_Suspect_1_Bank&gt; | 1st | &lt;Template_Suspect_1_Account_Number&gt;111-111111-101 &lt;/Template_Suspect_1_Account_Number&gt; | &lt;Template_Suspect_1_Name&gt;CHAN TAI MAN&lt;/Template_Suspect_1_Name&gt; |
+Transaction Details
+| S/N | Date | Currency | Involved Amounts | Approx. HKD | Remitting Bank | AC Location | Depositor AC No. | Depositor AC Name |
 | --- | ---- | -------- | ---------------- | ----------- | -------------- | ----------- | ---------------- | ----------------- |
-| 1 | 2024-08-24 | HKD | 50000 | 50000 | HSBC | Hong Kong | 444-4444444-101 | CHEUNG TAK SHING  |
-| 2 | 2024-08-25 | HKD | 10000 | 10000 | HSBC | Hong Kong | 444-4444444-101 | CHEUNG TAK SHING  |
-| 1 | 2024-08-24 | HKD | 31000 | 31000 | HSB | Hong Kong | 222-222222-101  | CHEUNG TAK SHING  |
-| 2 | 2024-08-25 | HKD | 50000 | 50000 | HSB | Hong Kong | 222-222222-101  | CHEUNG TAK SHING  |
-| 3 | 2024-08-25 | HKD | 60000 | 60000 | HSB | Hong Kong | 222-222222-101  | CHEUNG TAK SHING  |
-| 4 | 2024-08-25 | HKD | 30000 | 30000 | HSB | Hong Kong | 222-222222-101  | CHEUNG TAK SHING  |
-| 1 | 2024-08-25 | HKD | 39000 | 39000 | Hong Kong | CHEUNG TAK SHING  |</v>
-      </c>
-    </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A12" s="1"/>
-    </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A13" t="str">
-        <f>IF('ADCC-Params'!B6="Y","\*\*STR\*\*","\*\*NO STR\*\*")</f>
-        <v>\*\*NO STR\*\*</v>
-      </c>
-    </row>
-    <row r="15" spans="1:1" ht="78.75" x14ac:dyDescent="0.25">
-      <c r="A15" s="1" t="str">
+| 1 | &lt;Template_FraudPayment2_Date&gt;2024-08-24&lt;/Template_FraudPayment2_Date&gt; | &lt;Template_FraudPayment2_Currency&gt;HKD&lt;/Template_FraudPayment2_Currency&gt; | &lt;Template_FraudPayment2_Amount&gt;50000&lt;/Template_FraudPayment2_Amount&gt; | &lt;Template_FraudPayment2_Amount&gt;50000&lt;/Template_FraudPayment2_Amount&gt; | &lt;Template_Victim1_Account1_Bank&gt;HSBC&lt;/Template_Victim1_Account1_Bank&gt; | Hong Kong | &lt;Template_Victim1_Account1_AccountNumber&gt;444-4444444-101&lt;/Template_Victim1_Account1_AccountNumber&gt; | &lt;Template_Victim1_Name&gt;CHEUNG TAK SHING &lt;/Template_Victim1_Name&gt; |
+| 2 | &lt;Template_FraudPayment3_Date&gt;2024-08-25&lt;/Template_FraudPayment3_Date&gt; | &lt;Template_FraudPayment3_Currency&gt;HKD&lt;/Template_FraudPayment3_Currency&gt; | &lt;Template_FraudPayment3_Amount&gt;10000&lt;/Template_FraudPayment3_Amount&gt; | &lt;Template_FraudPayment3_Amount&gt;10000&lt;/Template_FraudPayment3_Amount&gt; | &lt;Template_Victim1_Account1_Bank&gt;HSBC&lt;/Template_Victim1_Account1_Bank&gt; | Hong Kong | &lt;Template_Victim1_Account1_AccountNumber&gt;444-4444444-101&lt;/Template_Victim1_Account1_AccountNumber&gt; | &lt;Template_Victim1_Name&gt;CHEUNG TAK SHING &lt;/Template_Victim1_Name&gt; |
+Transaction Details
+| S/N | Date | Currency | Involved Amounts | Approx. HKD | Remitting Bank | AC Location | Depositor AC No. | Depositor AC Name |
+| --- | ---- | -------- | ---------------- | ----------- | -------------- | ----------- | ---------------- | ----------------- |
+| 1 | &lt;Template_FraudPayment4_Date&gt;2024-08-24&lt;/Template_FraudPayment4_Date&gt; | &lt;Template_FraudPayment4_Currency&gt;HKD&lt;/Template_FraudPayment4_Currency&gt; | &lt;Template_FraudPayment4_Amount&gt;31000&lt;/Template_FraudPayment4_Amount&gt; | &lt;Template_FraudPayment4_Amount&gt;31000&lt;/Template_FraudPayment4_Amount&gt; | &lt;Template_Victim1_Account2_Bank&gt;HSB&lt;/Template_Victim1_Account2_Bank&gt; | Hong Kong | &lt;Template_Victim1_Account2_AccountNumber&gt;222-222222-101 &lt;/Template_Victim1_Account2_AccountNumber&gt; | &lt;Template_Victim1_Name&gt;CHEUNG TAK SHING &lt;/Template_Victim1_Name&gt; |
+| 2 | &lt;Template_FraudPayment5_Date&gt;2024-08-25&lt;/Template_FraudPayment5_Date&gt; | &lt;Template_FraudPayment5_Currency&gt;HKD&lt;/Template_FraudPayment5_Currency&gt; | &lt;Template_FraudPayment5_Amount&gt;50000&lt;/Template_FraudPayment5_Amount&gt; | &lt;Template_FraudPayment5_Amount&gt;50000&lt;/Template_FraudPayment5_Amount&gt; | &lt;Template_Victim1_Account2_Bank&gt;HSB&lt;/Template_Victim1_Account2_Bank&gt; | Hong Kong | &lt;Template_Victim1_Account2_AccountNumber&gt;222-222222-101 &lt;/Template_Victim1_Account2_AccountNumber&gt; | &lt;Template_Victim1_Name&gt;CHEUNG TAK SHING &lt;/Template_Victim1_Name&gt; |
+| 3 | &lt;Template_FraudPayment6_Date&gt;2024-08-25&lt;/Template_FraudPayment6_Date&gt; | &lt;Template_FraudPayment6_Currency&gt;HKD&lt;/Template_FraudPayment6_Currency&gt; | &lt;Template_FraudPayment6_Amount&gt;60000&lt;/Template_FraudPayment6_Amount&gt; | &lt;Template_FraudPayment6_Amount&gt;60000&lt;/Template_FraudPayment6_Amount&gt; | &lt;Template_Victim1_Account2_Bank&gt;HSB&lt;/Template_Victim1_Account2_Bank&gt; | Hong Kong | &lt;Template_Victim1_Account2_AccountNumber&gt;222-222222-101 &lt;/Template_Victim1_Account2_AccountNumber&gt; | &lt;Template_Victim1_Name&gt;CHEUNG TAK SHING &lt;/Template_Victim1_Name&gt; |
+| 4 | &lt;Template_FraudPayment7_Date&gt;2024-08-25&lt;/Template_FraudPayment7_Date&gt; | &lt;Template_FraudPayment7_Currency&gt;HKD&lt;/Template_FraudPayment7_Currency&gt; | &lt;Template_FraudPayment7_Amount&gt;30000&lt;/Template_FraudPayment7_Amount&gt; | &lt;Template_FraudPayment7_Amount&gt;30000&lt;/Template_FraudPayment7_Amount&gt; | &lt;Template_Victim1_Account2_Bank&gt;HSB&lt;/Template_Victim1_Account2_Bank&gt; | Hong Kong | &lt;Template_Victim1_Account2_AccountNumber&gt;222-222222-101 &lt;/Template_Victim1_Account2_AccountNumber&gt; | &lt;Template_Victim1_Name&gt;CHEUNG TAK SHING &lt;/Template_Victim1_Name&gt; |
+Transaction Details
+| S/N | Date | Currency | Involved Amounts | Approx. HKD | Remitting Bank | AC Location | Depositor AC No. | Depositor AC Name |
+| --- | ---- | -------- | ---------------- | ----------- | -------------- | ----------- | ---------------- | ----------------- |
+| 1 | &lt;Template_FraudPayment8_Date&gt;2024-08-25&lt;/Template_FraudPayment8_Date&gt; | &lt;Template_FraudPayment8_Currency&gt;HKD&lt;/Template_FraudPayment8_Currency&gt; | &lt;Template_FraudPayment8_Amount&gt;39000&lt;/Template_FraudPayment8_Amount&gt; | &lt;Template_FraudPayment8_Amount&gt;39000&lt;/Template_FraudPayment8_Amount&gt; | &lt;Template_Victim1_Account3_Bank&gt;&lt;/Template_Victim1_Account3_Bank&gt; | Hong Kong | &lt;Template_Victim1_Account3_AccountNumber&gt;&lt;/Template_Victim1_Account3_AccountNumber&gt; | &lt;Template_Victim1_Name&gt;CHEUNG TAK SHING &lt;/Template_Victim1_Name&gt; |
+\*\*NO STR\*\*
+Details of Beneficiary
+| Ref. | Beneficiary Bank | Layer | Beneficiary Account No. | Beneficiary Account Name |
+| ---- | ---------------- | ----- | ----------------------- | ------------------------ |
+| AC2 | &lt;Template_Suspect_2_Bank&gt;HSB&lt;/Template_Suspect_2_Bank&gt; | 1st | &lt;Template_Suspect_2_Account_Number&gt;111-111111-102 &lt;/Template_Suspect_2_Account_Number&gt; | &lt;Template_Suspect_2_Name&gt;CHUNG SIU&lt;/Template_Suspect_2_Name&gt; |
+Transaction Details
+| S/N | Date | Currency | Involved Amounts | Approx. HKD | Remitting Bank | AC Location | Depositor AC No. | Depositor AC Name |
+| --- | ---- | -------- | ---------------- | ----------- | -------------- | ----------- | ---------------- | ----------------- |
+| 1 | &lt;Template_FraudPayment9_Date&gt;2024-08-25&lt;/Template_FraudPayment9_Date&gt; | &lt;Template_FraudPayment9_Currency&gt;HKD&lt;/Template_FraudPayment9_Currency&gt; | &lt;Template_FraudPayment9_Amount&gt;50000&lt;/Template_FraudPayment9_Amount&gt; | &lt;Template_FraudPayment9_Amount&gt;50000&lt;/Template_FraudPayment9_Amount&gt; | &lt;Template_Victim1_Account1_Bank&gt;HSBC&lt;/Template_Victim1_Account1_Bank&gt; | Hong Kong | &lt;Template_Victim1_Account1_AccountNumber&gt;444-4444444-101&lt;/Template_Victim1_Account1_AccountNumber&gt; | &lt;Template_Victim1_Name&gt;CHEUNG TAK SHING &lt;/Template_Victim1_Name&gt; |
+Transaction Details
+| S/N | Date | Currency | Involved Amounts | Approx. HKD | Remitting Bank | AC Location | Depositor AC No. | Depositor AC Name |
+| --- | ---- | -------- | ---------------- | ----------- | -------------- | ----------- | ---------------- | ----------------- |
+| 1 | &lt;Template_FraudPayment10_Date&gt;2024-08-25&lt;/Template_FraudPayment10_Date&gt; | &lt;Template_FraudPayment10_Currency&gt;HKD&lt;/Template_FraudPayment10_Currency&gt; | &lt;Template_FraudPayment10_Amount&gt;50000&lt;/Template_FraudPayment10_Amount&gt; | &lt;Template_FraudPayment10_Amount&gt;50000&lt;/Template_FraudPayment10_Amount&gt; | &lt;Template_Victim1_Account2_Bank&gt;HSB&lt;/Template_Victim1_Account2_Bank&gt; | Hong Kong | &lt;Template_Victim1_Account2_AccountNumber&gt;222-222222-101 &lt;/Template_Victim1_Account2_AccountNumber&gt; | &lt;Template_Victim1_Name&gt;CHEUNG TAK SHING &lt;/Template_Victim1_Name&gt; |
+\*\*NO STR\*\*</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" ht="78.75" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="str">
         <f>'ADCC-Template'!B10&amp;"**"&amp;'ADCC-Params'!B7&amp;"**"&amp;'ADCC-Template'!B11&amp;"**"&amp;'ADCC-Params'!B8&amp;"** "&amp;'ADCC-Template'!B12&amp;"**"&amp;'ADCC-Params'!B9&amp;"** "&amp;'ADCC-Template'!B13</f>
         <v>We have examined each report referred by the subject investigation team and we believe that **the beneficiary account(s) might have been used to deal with suspected proceeds of crime**. Therefore, you are advised (i) **to critically examine the alleged transaction(s) in the relevant account(s)** to ascertain whether or not you are satisfied that the provenance of the deposits into the said account(s) is legitimate and (ii) **to actively consider appropriate actions** to avoid dealing with property in whole or in part directly or indirectly represent any person's proceeds of an indictable offence, which may be liable to a prosecution for a criminal offence under sections 25(1) and (3) of the Organized and Serious Crimes Ordinance, Cap. 455. A person includes a financial institution.</v>
       </c>
     </row>
-    <row r="17" spans="1:1" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A17" s="1" t="str">
-        <f>'ADCC-Template'!B14&amp;"**"&amp;"&lt;Template_Reporting_Reference&gt;"&amp;'ADCC-Params'!B10&amp;"&lt;/Template_Reporting_Reference&gt;"&amp;" ("&amp;'ADCC-Params'!B4&amp;")** "&amp;'ADCC-Template'!B15</f>
-        <v>When fulfilling the reporting obligations by filing Suspicious Transaction Reports (STR) to the Joint Financial Intelligence Unit ("JFIU"), if any, please state **&lt;Template_Reporting_Reference&gt;ESPS 7■■■■■■ and NTKDIV 24■■■■■&lt;/Template_Reporting_Reference&gt; (DIT2-■■■■■)** for ease of reference.</v>
-      </c>
-    </row>
-    <row r="19" spans="1:1" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A19" s="1" t="str">
+    <row r="12" spans="1:1" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="str">
+        <f>'ADCC-Template'!B14&amp;"**"&amp;"&lt;Template_ReportingReference&gt;"&amp;'ADCC-Params'!B10&amp;"&lt;/Template_ReportingReference&gt;"&amp;" ("&amp;'ADCC-Params'!B4&amp;")** "&amp;'ADCC-Template'!B15</f>
+        <v>When fulfilling the reporting obligations by filing Suspicious Transaction Reports (STR) to the Joint Financial Intelligence Unit ("JFIU"), if any, please state **&lt;Template_ReportingReference&gt;ESPS 7■■■■■■ and NTKDIV 24■■■■■&lt;/Template_ReportingReference&gt; (DIT2-■■■■■)** for ease of reference.</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="A14" s="1" t="str">
         <f>'ADCC-Template'!B16</f>
         <v>We confirm that the requested information is required for the purpose of section 58(1)(a) under the Personal Data (Privacy) Ordinance, Cap 486. Failure to provide the requested information may lead to possibly failure or unnecessary delay on prevention or detection of crime. In view of the above, we consider that section 58(2) as read with section 58(1)(a) of the Personal Data (Privacy) Ordinance, Cap. 486 is the applicable exemption under the circumstances.</v>
       </c>
     </row>
-    <row r="21" spans="1:1" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A21" s="1" t="str">
+    <row r="16" spans="1:1" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A16" s="1" t="str">
         <f>'ADCC-Template'!B17</f>
         <v>You are also advised to refer to the "Guideline on Anti-Money Laundering and Counter-Terrorist Financing" published by the Hong Kong Monetary Authority (HKMA) under the Anti-Money Laundering and Counter-Terrorist Financing (Financial Institutions) Ordinance, Cap. 615 ("AMLO") and to take all reasonable measures to prevent a contravention and to mitigate Money Laundering risks.</v>
       </c>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A23" t="str">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A18" t="str">
         <f>'ADCC-Template'!B18&amp;'ADCC-Params'!B11&amp;'ADCC-Template'!B19</f>
         <v xml:space="preserve">Should you have any enquiry, please feel free to contact the undersigned or our officers at 286■■■■■. Thank you! </v>
       </c>
     </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A25" t="str">
+    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A20" t="str">
         <f>'ADCC-Template'!B20</f>
         <v xml:space="preserve">Best regards, </v>
       </c>
     </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A26" s="2" t="str">
+    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A21" s="2" t="str">
         <f>'ADCC-Params'!B12</f>
         <v xml:space="preserve">PC 15■■■ Sze-yuen </v>
       </c>
     </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A27" t="str">
+    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A22" t="str">
         <f>'ADCC-Template'!B21</f>
         <v>Anti-Deception Coordination Centre 
 Commercial Crime Bureau 
 Hong Kong Police Force</v>
       </c>
     </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A28" t="str">
+    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A23" t="str">
         <f>"Tel: "&amp;'ADCC-Params'!B11&amp;" / Fax: "&amp;'ADCC-Params'!B13</f>
         <v>Tel: 286■■■■■ / Fax: 220■■■■■</v>
       </c>

</xml_diff>